<commit_message>
Update statistics for board report
</commit_message>
<xml_diff>
--- a/statistics_files/nekls_executive_board/2022/2022.02.next_search_catalog.xlsx
+++ b/statistics_files/nekls_executive_board/2022/2022.02.next_search_catalog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\nekls_executive_board\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FC9CDB-3068-4281-AC9C-5F50FEB08DD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAC0FB8-B91A-4299-86C4-157882ACF6ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" xr2:uid="{4F58177C-A508-401B-B121-B6C236B4EE04}"/>
   </bookViews>
@@ -335,70 +335,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,12 +719,12 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:D1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" style="22" customWidth="1"/>
     <col min="2" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -732,481 +732,823 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="5">
+        <v>10674</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1588</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2187</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="7">
+        <v>4708</v>
+      </c>
+      <c r="C4" s="7">
+        <v>665</v>
+      </c>
+      <c r="D4" s="7">
+        <v>754</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="5">
+        <v>17260</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1389</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1866</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="7">
+        <v>211</v>
+      </c>
+      <c r="C6" s="7">
+        <v>141</v>
+      </c>
+      <c r="D6" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="5">
+        <v>10279</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2274</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1875</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="7">
+        <v>1341</v>
+      </c>
+      <c r="C8" s="7">
+        <v>271</v>
+      </c>
+      <c r="D8" s="7">
+        <v>283</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="5">
+        <v>1561</v>
+      </c>
+      <c r="C9" s="5">
+        <v>263</v>
+      </c>
+      <c r="D9" s="5">
+        <v>270</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7">
+        <v>426</v>
+      </c>
+      <c r="C10" s="7">
+        <v>93</v>
+      </c>
+      <c r="D10" s="7">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="5">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="9">
+        <v>242</v>
+      </c>
+      <c r="C13" s="9">
+        <v>90</v>
+      </c>
+      <c r="D13" s="9">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="11">
+        <v>639</v>
+      </c>
+      <c r="C14" s="11">
+        <v>407</v>
+      </c>
+      <c r="D14" s="11">
+        <v>400</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="9">
+        <v>1195</v>
+      </c>
+      <c r="C15" s="9">
+        <v>646</v>
+      </c>
+      <c r="D15" s="9">
+        <v>302</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="11">
+        <v>866</v>
+      </c>
+      <c r="C16" s="11">
+        <v>463</v>
+      </c>
+      <c r="D16" s="11">
+        <v>272</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="5">
+        <v>417</v>
+      </c>
+      <c r="C17" s="5">
+        <v>176</v>
+      </c>
+      <c r="D17" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7">
+        <v>3829</v>
+      </c>
+      <c r="C18" s="7">
+        <v>704</v>
+      </c>
+      <c r="D18" s="7">
+        <v>848</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="5">
+        <v>781</v>
+      </c>
+      <c r="C19" s="5">
+        <v>212</v>
+      </c>
+      <c r="D19" s="5">
+        <v>160</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="B20" s="7">
+        <v>5172</v>
+      </c>
+      <c r="C20" s="7">
+        <v>612</v>
+      </c>
+      <c r="D20" s="7">
+        <v>970</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="5">
+        <v>90</v>
+      </c>
+      <c r="C21" s="5">
+        <v>112</v>
+      </c>
+      <c r="D21" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="B22" s="7">
+        <v>4976</v>
+      </c>
+      <c r="C22" s="7">
+        <v>498</v>
+      </c>
+      <c r="D22" s="7">
+        <v>879</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="5">
+        <v>243</v>
+      </c>
+      <c r="C23" s="5">
+        <v>147</v>
+      </c>
+      <c r="D23" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="B24" s="7">
+        <v>3779</v>
+      </c>
+      <c r="C24" s="7">
+        <v>740</v>
+      </c>
+      <c r="D24" s="7">
+        <v>877</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="5">
+        <v>16657</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2257</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
+      <c r="B26" s="7">
+        <v>1264</v>
+      </c>
+      <c r="C26" s="7">
+        <v>395</v>
+      </c>
+      <c r="D26" s="7">
+        <v>196</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="B28" s="7">
+        <v>1335</v>
+      </c>
+      <c r="C28" s="7">
+        <v>320</v>
+      </c>
+      <c r="D28" s="7">
+        <v>341</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="5">
+        <v>690</v>
+      </c>
+      <c r="C29" s="5">
+        <v>101</v>
+      </c>
+      <c r="D29" s="5">
+        <v>154</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="B30" s="7">
+        <v>3642</v>
+      </c>
+      <c r="C30" s="7">
+        <v>816</v>
+      </c>
+      <c r="D30" s="7">
+        <v>710</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="5">
+        <v>156</v>
+      </c>
+      <c r="C31" s="5">
+        <v>72</v>
+      </c>
+      <c r="D31" s="5">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="B32" s="7">
+        <v>473</v>
+      </c>
+      <c r="C32" s="7">
+        <v>450</v>
+      </c>
+      <c r="D32" s="7">
+        <v>69</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="B33" s="5">
+        <v>3991</v>
+      </c>
+      <c r="C33" s="5">
+        <v>836</v>
+      </c>
+      <c r="D33" s="5">
+        <v>788</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="B34" s="7">
+        <v>3014</v>
+      </c>
+      <c r="C34" s="7">
+        <v>704</v>
+      </c>
+      <c r="D34" s="7">
+        <v>844</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="B35" s="5">
+        <v>1540</v>
+      </c>
+      <c r="C35" s="5">
+        <v>240</v>
+      </c>
+      <c r="D35" s="5">
+        <v>396</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="B36" s="7">
+        <v>11501</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1390</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1521</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="B37" s="5">
+        <v>2244</v>
+      </c>
+      <c r="C37" s="5">
+        <v>755</v>
+      </c>
+      <c r="D37" s="5">
+        <v>404</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="B38" s="7">
+        <v>4112</v>
+      </c>
+      <c r="C38" s="7">
+        <v>535</v>
+      </c>
+      <c r="D38" s="7">
+        <v>765</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="B39" s="5">
+        <v>207</v>
+      </c>
+      <c r="C39" s="5">
+        <v>188</v>
+      </c>
+      <c r="D39" s="5">
+        <v>42</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="B40" s="7">
+        <v>331</v>
+      </c>
+      <c r="C40" s="7">
+        <v>65</v>
+      </c>
+      <c r="D40" s="7">
+        <v>83</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+      <c r="B41" s="13">
+        <v>871</v>
+      </c>
+      <c r="C41" s="13">
+        <v>126</v>
+      </c>
+      <c r="D41" s="13">
+        <v>85</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="B42" s="15">
+        <v>4391</v>
+      </c>
+      <c r="C42" s="15">
+        <v>185</v>
+      </c>
+      <c r="D42" s="15">
+        <v>109</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
+      <c r="B43" s="13">
+        <v>173</v>
+      </c>
+      <c r="C43" s="13">
+        <v>55</v>
+      </c>
+      <c r="D43" s="13">
+        <v>62</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
+      <c r="B44" s="15">
+        <v>261</v>
+      </c>
+      <c r="C44" s="15">
+        <v>39</v>
+      </c>
+      <c r="D44" s="15">
+        <v>13</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
+      <c r="B45" s="13">
+        <v>866</v>
+      </c>
+      <c r="C45" s="13">
+        <v>90</v>
+      </c>
+      <c r="D45" s="13">
+        <v>26</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="B46" s="7">
+        <v>709</v>
+      </c>
+      <c r="C46" s="7">
+        <v>226</v>
+      </c>
+      <c r="D46" s="7">
+        <v>115</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+      <c r="B47" s="5">
+        <v>3049</v>
+      </c>
+      <c r="C47" s="5">
+        <v>844</v>
+      </c>
+      <c r="D47" s="5">
+        <v>559</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="B48" s="7">
+        <v>7617</v>
+      </c>
+      <c r="C48" s="7">
+        <v>887</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1403</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="B49" s="5">
+        <v>3035</v>
+      </c>
+      <c r="C49" s="5">
+        <v>946</v>
+      </c>
+      <c r="D49" s="5">
+        <v>314</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
+      <c r="B50" s="7">
+        <v>2537</v>
+      </c>
+      <c r="C50" s="7">
+        <v>294</v>
+      </c>
+      <c r="D50" s="7">
+        <v>504</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
+      <c r="B51" s="5">
+        <v>5775</v>
+      </c>
+      <c r="C51" s="5">
+        <v>826</v>
+      </c>
+      <c r="D51" s="5">
+        <v>909</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
+      <c r="B52" s="7">
+        <v>1060</v>
+      </c>
+      <c r="C52" s="7">
+        <v>128</v>
+      </c>
+      <c r="D52" s="7">
+        <v>212</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="B53" s="5">
+        <v>3157</v>
+      </c>
+      <c r="C53" s="5">
+        <v>797</v>
+      </c>
+      <c r="D53" s="5">
+        <v>737</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+      <c r="B54" s="7">
+        <v>521</v>
+      </c>
+      <c r="C54" s="7">
+        <v>189</v>
+      </c>
+      <c r="D54" s="7">
+        <v>360</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="B55" s="5">
+        <v>380</v>
+      </c>
+      <c r="C55" s="5">
+        <v>362</v>
+      </c>
+      <c r="D55" s="5">
+        <v>81</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+      <c r="B56" s="7">
+        <v>950</v>
+      </c>
+      <c r="C56" s="7">
+        <v>273</v>
+      </c>
+      <c r="D56" s="7">
+        <v>444</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
+      <c r="B57" s="17">
+        <v>2942</v>
+      </c>
+      <c r="C57" s="17">
+        <v>1606</v>
+      </c>
+      <c r="D57" s="17">
+        <v>1056</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
+      <c r="B58" s="19">
+        <v>6562</v>
+      </c>
+      <c r="C58" s="19">
+        <v>495</v>
+      </c>
+      <c r="D58" s="19">
+        <v>295</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
+      <c r="B59" s="21">
+        <v>155212</v>
+      </c>
+      <c r="C59" s="21">
+        <v>26702</v>
+      </c>
+      <c r="D59" s="21">
+        <v>26702</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D59" xr:uid="{6CA45A21-3256-46F4-A196-E6610455B173}"/>

</xml_diff>